<commit_message>
intial fred dashboard implemented
</commit_message>
<xml_diff>
--- a/reference/fred.xlsx
+++ b/reference/fred.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0262c379d83082fb/Desktop/Code/BG_Mono/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_F25DC773A252ABDACC104895C19E7EF25ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC7C9AFA-44E3-498F-B115-342129CE4476}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_F25DC773A252ABDACC104895C19E7EF25ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A390FC03-F6C4-4D87-8E6C-0CEC16205CE2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>fred_id</t>
   </si>
@@ -56,81 +56,54 @@
     <t>GS10</t>
   </si>
   <si>
-    <t>10-Year Treasury</t>
-  </si>
-  <si>
     <t>10-Year Treasury Yield</t>
   </si>
   <si>
     <t>DFII10</t>
   </si>
   <si>
-    <t>10-Year TIPS Yield</t>
-  </si>
-  <si>
     <t>10-Year Real TIPS Yield</t>
   </si>
   <si>
     <t>FEDFUNDS</t>
   </si>
   <si>
-    <t>Federal Funds Rate</t>
-  </si>
-  <si>
     <t>Fed Funds Rate</t>
   </si>
   <si>
     <t>CPIAUCSL</t>
   </si>
   <si>
-    <t>CPI</t>
-  </si>
-  <si>
     <t>Consumer Price Index</t>
   </si>
   <si>
     <t>PCEPI</t>
   </si>
   <si>
-    <t>PCE</t>
-  </si>
-  <si>
     <t>Personal Consumption Expenditures</t>
   </si>
   <si>
     <t>CPILFESL</t>
   </si>
   <si>
-    <t>Core CPI</t>
-  </si>
-  <si>
     <t>Core Consumer Price Index</t>
   </si>
   <si>
     <t>PCEPILFE</t>
   </si>
   <si>
-    <t>Core PCE</t>
-  </si>
-  <si>
     <t>Core Personal Consumption Expenditures</t>
   </si>
   <si>
     <t>GDP</t>
   </si>
   <si>
-    <t>Nominal GDP</t>
-  </si>
-  <si>
     <t>Gross Domestic Product (Nominal)</t>
   </si>
   <si>
     <t>GDPC1</t>
   </si>
   <si>
-    <t>Real GDP</t>
-  </si>
-  <si>
     <t>Gross Domestic Product (Real)</t>
   </si>
   <si>
@@ -143,81 +116,54 @@
     <t>CIVPART</t>
   </si>
   <si>
-    <t>Labor Participation Rate</t>
-  </si>
-  <si>
     <t>Labor Force Participation Rate</t>
   </si>
   <si>
     <t>PSAVERT</t>
   </si>
   <si>
-    <t>Personal Savings Rate</t>
-  </si>
-  <si>
     <t>Personal Saving Rate</t>
   </si>
   <si>
     <t>PAYEMS</t>
   </si>
   <si>
-    <t>Nonfarm Payrolls</t>
-  </si>
-  <si>
     <t>Total Nonfarm Payroll Employment</t>
   </si>
   <si>
     <t>ICSA</t>
   </si>
   <si>
-    <t>Initial Jobless Claims</t>
-  </si>
-  <si>
     <t>Initial Unemployment Claims</t>
   </si>
   <si>
     <t>UMCSENT</t>
   </si>
   <si>
-    <t>Michigan Consumer Sentiment</t>
-  </si>
-  <si>
     <t>Consumer Sentiment Index</t>
   </si>
   <si>
     <t>DSPIC96</t>
   </si>
   <si>
-    <t>Real Disposable Income</t>
-  </si>
-  <si>
     <t>Real Disposable Personal Income</t>
   </si>
   <si>
     <t>RRSFS</t>
   </si>
   <si>
-    <t>Retail Sales</t>
-  </si>
-  <si>
     <t>Retail and Food Services Sales</t>
   </si>
   <si>
     <t>INDPRO</t>
   </si>
   <si>
-    <t>Industrial Production</t>
-  </si>
-  <si>
     <t>Industrial Production Index</t>
   </si>
   <si>
     <t>TCU</t>
   </si>
   <si>
-    <t>Capacity Utilization</t>
-  </si>
-  <si>
     <t>Capacity Utilization: Total Industry</t>
   </si>
   <si>
@@ -231,6 +177,72 @@
   </si>
   <si>
     <t>ISM Manufacturing PMI</t>
+  </si>
+  <si>
+    <t>10_year_treasury</t>
+  </si>
+  <si>
+    <t>10_year_tips_yield</t>
+  </si>
+  <si>
+    <t>federal_funds_rate</t>
+  </si>
+  <si>
+    <t>cpi</t>
+  </si>
+  <si>
+    <t>pce</t>
+  </si>
+  <si>
+    <t>core_cpi</t>
+  </si>
+  <si>
+    <t>core_pce</t>
+  </si>
+  <si>
+    <t>nominal_gdp</t>
+  </si>
+  <si>
+    <t>real_gdp</t>
+  </si>
+  <si>
+    <t>unemployment_rate</t>
+  </si>
+  <si>
+    <t>labor_participation_rate</t>
+  </si>
+  <si>
+    <t>personal_savings_rate</t>
+  </si>
+  <si>
+    <t>nonfarm_payrolls</t>
+  </si>
+  <si>
+    <t>initial_jobless_claims</t>
+  </si>
+  <si>
+    <t>michigan_consumer_sentiment</t>
+  </si>
+  <si>
+    <t>real_disposable_income</t>
+  </si>
+  <si>
+    <t>retail_sales</t>
+  </si>
+  <si>
+    <t>industrial_production</t>
+  </si>
+  <si>
+    <t>capacity_utilization</t>
+  </si>
+  <si>
+    <t>housing_starts</t>
+  </si>
+  <si>
+    <t>ism_manufacturing_pmi</t>
+  </si>
+  <si>
+    <t>dashboard_1</t>
   </si>
 </sst>
 </file>
@@ -568,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,11 +591,10 @@
     <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,327 +610,389 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2" s="2" t="str">
         <f>HYPERLINK("https://fred.stlouisfed.org/series/"&amp;A2)</f>
         <v>https://fred.stlouisfed.org/series/GS10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
       </c>
       <c r="D3" s="2" t="str">
         <f t="shared" ref="D3:D22" si="0">HYPERLINK("https://fred.stlouisfed.org/series/"&amp;A3)</f>
         <v>https://fred.stlouisfed.org/series/DFII10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/FEDFUNDS</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/CPIAUCSL</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/FEDFUNDS</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/PCEPI</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/CPIAUCSL</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="D7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/CPILFESL</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/PCEPILFE</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/PCEPI</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/GDP</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/CPILFESL</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="D10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/GDPC1</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/UNRATE</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/PCEPILFE</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/CIVPART</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/GDP</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="D13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/PSAVERT</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/PAYEMS</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/GDPC1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/ICSA</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>33</v>
       </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/UNRATE</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
         <v>34</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/UMCSENT</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>35</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/CIVPART</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="D17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/DSPIC96</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>37</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" t="s">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/RRSFS</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/PSAVERT</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
         <v>40</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/INDPRO</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>41</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/PAYEMS</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="D20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/TCU</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
         <v>44</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/HOUST</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/ICSA</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
         <v>46</v>
       </c>
-      <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/UMCSENT</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/DSPIC96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/RRSFS</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/INDPRO</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/TCU</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/HOUST</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" t="s">
-        <v>64</v>
-      </c>
       <c r="D22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://fred.stlouisfed.org/series/NAPM</v>
       </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://fred.stlouisfed.org/series/GS10" xr:uid="{B424553A-A170-41BE-B292-910589049E5C}"/>
-    <hyperlink ref="D3:D22" r:id="rId2" display="https://fred.stlouisfed.org/series/GS10" xr:uid="{7E64F40C-32CC-4B23-B1A8-E85F654312E8}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completed basic formatting for macro dashboard
</commit_message>
<xml_diff>
--- a/reference/fred.xlsx
+++ b/reference/fred.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0262c379d83082fb/Desktop/Code/BG_Mono/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_F25DC773A252ABDACC104895C19E7EF25ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A390FC03-F6C4-4D87-8E6C-0CEC16205CE2}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="11_F25DC773A252ABDACC104895C19E7EF25ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2795A5CD-F8E6-48FB-BB3E-C4FBE56ED6E9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>fred_id</t>
   </si>
@@ -53,9 +53,6 @@
     <t>notes</t>
   </si>
   <si>
-    <t>GS10</t>
-  </si>
-  <si>
     <t>10-Year Treasury Yield</t>
   </si>
   <si>
@@ -173,12 +170,6 @@
     <t>Housing Starts</t>
   </si>
   <si>
-    <t>NAPM</t>
-  </si>
-  <si>
-    <t>ISM Manufacturing PMI</t>
-  </si>
-  <si>
     <t>10_year_treasury</t>
   </si>
   <si>
@@ -239,10 +230,22 @@
     <t>housing_starts</t>
   </si>
   <si>
-    <t>ism_manufacturing_pmi</t>
-  </si>
-  <si>
     <t>dashboard_1</t>
+  </si>
+  <si>
+    <t>DGS10</t>
+  </si>
+  <si>
+    <t>decimals</t>
+  </si>
+  <si>
+    <t>show_percent</t>
+  </si>
+  <si>
+    <t>show_dollar</t>
+  </si>
+  <si>
+    <t>use_commas</t>
   </si>
 </sst>
 </file>
@@ -580,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G1" sqref="G1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,9 +595,14 @@
     <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,361 +619,601 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
       <c r="D2" s="2" t="str">
         <f>HYPERLINK("https://fred.stlouisfed.org/series/"&amp;A2)</f>
-        <v>https://fred.stlouisfed.org/series/GS10</v>
+        <v>https://fred.stlouisfed.org/series/DGS10</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" s="2" t="str">
+        <f t="shared" ref="D3:D21" si="0">HYPERLINK("https://fred.stlouisfed.org/series/"&amp;A3)</f>
+        <v>https://fred.stlouisfed.org/series/DFII10</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/FEDFUNDS</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/CPIAUCSL</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="str">
-        <f t="shared" ref="D3:D22" si="0">HYPERLINK("https://fred.stlouisfed.org/series/"&amp;A3)</f>
-        <v>https://fred.stlouisfed.org/series/DFII10</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/PCEPI</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
         <v>49</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/FEDFUNDS</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/CPILFESL</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>50</v>
       </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/CPIAUCSL</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/PCEPILFE</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
         <v>51</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/PCEPI</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/GDP</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
         <v>52</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/CPILFESL</v>
-      </c>
-      <c r="F7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/GDPC1</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
         <v>53</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/PCEPILFE</v>
-      </c>
-      <c r="F8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/UNRATE</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
         <v>54</v>
       </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/GDP</v>
-      </c>
-      <c r="F9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/CIVPART</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
         <v>55</v>
       </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/GDPC1</v>
-      </c>
-      <c r="F10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/PSAVERT</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
         <v>56</v>
       </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/UNRATE</v>
-      </c>
-      <c r="F11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/PAYEMS</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
         <v>57</v>
       </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/CIVPART</v>
-      </c>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/ICSA</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
         <v>58</v>
       </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/PSAVERT</v>
-      </c>
-      <c r="F13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/UMCSENT</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
         <v>59</v>
       </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/PAYEMS</v>
-      </c>
-      <c r="F14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/DSPIC96</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
         <v>60</v>
       </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/ICSA</v>
-      </c>
-      <c r="F15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/RRSFS</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
         <v>61</v>
       </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/UMCSENT</v>
-      </c>
-      <c r="F16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/INDPRO</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
         <v>62</v>
       </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/DSPIC96</v>
-      </c>
-      <c r="F17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>https://fred.stlouisfed.org/series/TCU</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
         <v>63</v>
       </c>
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/RRSFS</v>
-      </c>
-      <c r="F18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/INDPRO</v>
-      </c>
-      <c r="F19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/TCU</v>
-      </c>
-      <c r="F20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="C21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" t="s">
-        <v>44</v>
-      </c>
       <c r="D21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>https://fred.stlouisfed.org/series/HOUST</v>
@@ -973,26 +1221,21 @@
       <c r="F21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>https://fred.stlouisfed.org/series/NAPM</v>
-      </c>
-      <c r="F22" t="b">
-        <v>1</v>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sometimes I just amaze myself
</commit_message>
<xml_diff>
--- a/reference/fred.xlsx
+++ b/reference/fred.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0262c379d83082fb/Desktop/Code/BG_Mono/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="11_F25DC773A252ABDACC104895C19E7EF25ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2795A5CD-F8E6-48FB-BB3E-C4FBE56ED6E9}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="11_F25DC773A252ABDACC104895C19E7EF25ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{549B3815-024B-4984-A8DA-B70E11F80C7D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -586,7 +586,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:J1"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1012,10 +1012,10 @@
         <v>1</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
@@ -1042,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
@@ -1132,7 +1132,7 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
@@ -1195,7 +1195,7 @@
         <v>2</v>
       </c>
       <c r="H20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
@@ -1222,7 +1222,7 @@
         <v>1</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
inflation chart looking ok
</commit_message>
<xml_diff>
--- a/reference/fred.xlsx
+++ b/reference/fred.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0262c379d83082fb/Desktop/Code/BG_Mono/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="11_F25DC773A252ABDACC104895C19E7EF25ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{549B3815-024B-4984-A8DA-B70E11F80C7D}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="11_F25DC773A252ABDACC104895C19E7EF25ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F221A9B-1E66-49C4-9E5F-6211A8428DC3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -586,7 +586,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
launch file on completion of scrip
</commit_message>
<xml_diff>
--- a/reference/fred.xlsx
+++ b/reference/fred.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0262c379d83082fb/Desktop/Code/BG_Mono/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="11_F25DC773A252ABDACC104895C19E7EF25ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F14A5A63-5842-4E55-AF3E-27761573B840}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="11_F25DC773A252ABDACC104895C19E7EF25ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A77EB711-2F7E-4B8E-8BAC-C375FE87A3B1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,9 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -779,7 +777,7 @@
         <v>https://fred.stlouisfed.org/series/CPIAUCSL</v>
       </c>
       <c r="G5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -812,7 +810,7 @@
         <v>https://fred.stlouisfed.org/series/PCEPI</v>
       </c>
       <c r="G6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -845,7 +843,7 @@
         <v>https://fred.stlouisfed.org/series/CPILFESL</v>
       </c>
       <c r="G7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -878,7 +876,7 @@
         <v>https://fred.stlouisfed.org/series/PCEPILFE</v>
       </c>
       <c r="G8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>2</v>

</xml_diff>